<commit_message>
Add more missing observation cases
</commit_message>
<xml_diff>
--- a/Dataset missing_obs.xlsx
+++ b/Dataset missing_obs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sigve Borgmo\OneDrive - NTNU\Indok\Master\dynamic-factor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E375C77-7CBE-4AE9-8D3D-99719261F1E0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84C0BB2-9C1E-45E4-9827-45910E992BB8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{6A333D86-0EFE-48C5-877A-6581EBDEDD92}"/>
   </bookViews>
@@ -896,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C9044B-3D19-4C94-8316-B818C46B26B9}">
   <dimension ref="A1:BC273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM65" workbookViewId="0">
-      <selection activeCell="AN68" sqref="AN68:AN71"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1437,7 +1437,7 @@
         <v>3003.26189506836</v>
       </c>
       <c r="L4" s="1">
-        <v>94.775001525878906</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1">
         <v>445.36454545454501</v>
@@ -1604,7 +1604,7 @@
         <v>2870.45015814514</v>
       </c>
       <c r="L5" s="1">
-        <v>99.962501525878906</v>
+        <v>0</v>
       </c>
       <c r="M5" s="1">
         <v>467.27772499999998</v>
@@ -1616,7 +1616,7 @@
         <v>91.421051025390597</v>
       </c>
       <c r="P5" s="1">
-        <v>12.27</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="1">
         <v>117.55999756</v>
@@ -1771,7 +1771,7 @@
         <v>2919.6739780487101</v>
       </c>
       <c r="L6" s="1">
-        <v>110.47499847412099</v>
+        <v>0</v>
       </c>
       <c r="M6" s="1">
         <v>480.20130434782601</v>
@@ -1783,7 +1783,7 @@
         <v>97.951087951660199</v>
       </c>
       <c r="P6" s="1">
-        <v>12.27</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="1">
         <v>117.12000275</v>
@@ -1938,7 +1938,7 @@
         <v>2894.8888229644799</v>
       </c>
       <c r="L7" s="1">
-        <v>113.22499847412099</v>
+        <v>0</v>
       </c>
       <c r="M7" s="1">
         <v>482.68200000000002</v>
@@ -1950,7 +1950,7 @@
         <v>102.315788269043</v>
       </c>
       <c r="P7" s="1">
-        <v>12.27</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="1">
         <v>115.25608826</v>
@@ -2105,7 +2105,7 @@
         <v>2771.57125569763</v>
       </c>
       <c r="L8" s="1">
-        <v>115.84999847412099</v>
+        <v>0</v>
       </c>
       <c r="M8" s="1">
         <v>476.58521739130401</v>
@@ -2117,7 +2117,7 @@
         <v>99.613639831542997</v>
       </c>
       <c r="P8" s="1">
-        <v>12.27</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="1">
         <v>111.98818970000001</v>
@@ -2272,7 +2272,7 @@
         <v>2987.6819434875501</v>
       </c>
       <c r="L9" s="1">
-        <v>104.357498168945</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1">
         <v>478.93636363636398</v>
@@ -2284,7 +2284,7 @@
         <v>92.431816101074205</v>
       </c>
       <c r="P9" s="1">
-        <v>12.27</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="1">
         <v>112.18618011</v>
@@ -2439,7 +2439,7 @@
         <v>3076.4500581665002</v>
       </c>
       <c r="L10" s="1">
-        <v>95.977073669433594</v>
+        <v>0</v>
       </c>
       <c r="M10" s="1">
         <v>539.09371428571399</v>
@@ -2451,7 +2451,7 @@
         <v>85.712501525878906</v>
       </c>
       <c r="P10" s="1">
-        <v>12.27</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="1">
         <v>107.85481262</v>
@@ -2606,7 +2606,7 @@
         <v>3040.1361964141802</v>
       </c>
       <c r="L11" s="1">
-        <v>84.650001525878906</v>
+        <v>0</v>
       </c>
       <c r="M11" s="1">
         <v>532.67060869565205</v>
@@ -2618,7 +2618,7 @@
         <v>82.456520080566406</v>
       </c>
       <c r="P11" s="1">
-        <v>12.27</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="1">
         <v>105.71755219000001</v>
@@ -2773,7 +2773,7 @@
         <v>2910.4250427642801</v>
       </c>
       <c r="L12" s="1">
-        <v>91.099998474121094</v>
+        <v>0</v>
       </c>
       <c r="M12" s="1">
         <v>542.87457142857102</v>
@@ -2785,7 +2785,7 @@
         <v>82.428573608398395</v>
       </c>
       <c r="P12" s="1">
-        <v>12.27</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="1">
         <v>105.06999969</v>
@@ -2940,7 +2940,7 @@
         <v>2810.0681743179298</v>
       </c>
       <c r="L13" s="1">
-        <v>91.525001525878906</v>
+        <v>0</v>
       </c>
       <c r="M13" s="1">
         <v>552.42250000000001</v>
@@ -2952,7 +2952,7 @@
         <v>82.204544067382798</v>
       </c>
       <c r="P13" s="1">
-        <v>12.27</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="1">
         <v>113.40000153</v>
@@ -3107,7 +3107,7 @@
         <v>2981.6190366485598</v>
       </c>
       <c r="L14" s="1">
-        <v>89.287498474121094</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1">
         <v>614.50836363636404</v>
@@ -3119,7 +3119,7 @@
         <v>77.964286804199205</v>
       </c>
       <c r="P14" s="1">
-        <v>12.27</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="1">
         <v>117.15000153</v>
@@ -3274,7 +3274,7 @@
         <v>2918.21064537659</v>
       </c>
       <c r="L15" s="1">
-        <v>88.425003051757798</v>
+        <v>0</v>
       </c>
       <c r="M15" s="1">
         <v>645.03977142857104</v>
@@ -3286,7 +3286,7 @@
         <v>73.046051025390597</v>
       </c>
       <c r="P15" s="1">
-        <v>12.27</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="1">
         <v>114.98217773</v>
@@ -3441,7 +3441,7 @@
         <v>2604.9999294311501</v>
       </c>
       <c r="L16" s="1">
-        <v>85.912498474121094</v>
+        <v>0</v>
       </c>
       <c r="M16" s="1">
         <v>694.66290434782604</v>
@@ -3608,7 +3608,7 @@
         <v>2544.66672335968</v>
       </c>
       <c r="L17" s="1">
-        <v>86.787498474121094</v>
+        <v>0</v>
       </c>
       <c r="M17" s="1">
         <v>705.53830000000005</v>
@@ -3620,7 +3620,7 @@
         <v>75.127502441406307</v>
       </c>
       <c r="P17" s="1">
-        <v>12.97</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="1">
         <v>114.94999695</v>
@@ -3787,7 +3787,7 @@
         <v>77.988098144531307</v>
       </c>
       <c r="P18" s="1">
-        <v>12.97</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="1">
         <v>118.49285125999999</v>
@@ -3954,7 +3954,7 @@
         <v>84.657501220703097</v>
       </c>
       <c r="P19" s="1">
-        <v>12.97</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="1">
         <v>134.94596863000001</v>
@@ -4121,7 +4121,7 @@
         <v>87.556816101074205</v>
       </c>
       <c r="P20" s="1">
-        <v>12.97</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="1">
         <v>146.11549377</v>
@@ -4139,7 +4139,7 @@
         <v>203.99893188476599</v>
       </c>
       <c r="V20" s="1">
-        <v>2.6899998982747402</v>
+        <v>0</v>
       </c>
       <c r="W20" s="1">
         <v>3.82</v>
@@ -4288,7 +4288,7 @@
         <v>82.1484375</v>
       </c>
       <c r="P21" s="1">
-        <v>12.97</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="1">
         <v>153.45387267999999</v>
@@ -4306,7 +4306,7 @@
         <v>196.63931274414099</v>
       </c>
       <c r="V21" s="1">
-        <v>2.6899998982747402</v>
+        <v>0</v>
       </c>
       <c r="W21" s="1">
         <v>3.79</v>
@@ -4455,7 +4455,7 @@
         <v>89.642860412597699</v>
       </c>
       <c r="P22" s="1">
-        <v>12.97</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="1">
         <v>151.62037659000001</v>
@@ -4473,7 +4473,7 @@
         <v>197.61999511718801</v>
       </c>
       <c r="V22" s="1">
-        <v>2.6899998982747402</v>
+        <v>0</v>
       </c>
       <c r="W22" s="1">
         <v>3.79</v>
@@ -4622,7 +4622,7 @@
         <v>96.090911865234403</v>
       </c>
       <c r="P23" s="1">
-        <v>12.97</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="1">
         <v>151.21353149000001</v>
@@ -4640,7 +4640,7 @@
         <v>186.820068359375</v>
       </c>
       <c r="V23" s="1">
-        <v>2.6899998982747402</v>
+        <v>0</v>
       </c>
       <c r="W23" s="1">
         <v>3.87</v>
@@ -4789,7 +4789,7 @@
         <v>98.912498474121094</v>
       </c>
       <c r="P24" s="1">
-        <v>12.97</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="1">
         <v>154.70500182999999</v>
@@ -4807,7 +4807,7 @@
         <v>145.239181518555</v>
       </c>
       <c r="V24" s="1">
-        <v>2.6899998982747402</v>
+        <v>0</v>
       </c>
       <c r="W24" s="1">
         <v>3.81</v>
@@ -4956,7 +4956,7 @@
         <v>101.510871887207</v>
       </c>
       <c r="P25" s="1">
-        <v>12.97</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="1">
         <v>159.63999939000001</v>
@@ -5123,7 +5123,7 @@
         <v>89.970001220703097</v>
       </c>
       <c r="P26" s="1">
-        <v>12.97</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="1">
         <v>170.22599792</v>
@@ -5290,7 +5290,7 @@
         <v>90.685714721679702</v>
       </c>
       <c r="P27" s="1">
-        <v>12.97</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="1">
         <v>173.94999695000001</v>

</xml_diff>